<commit_message>
16/03/2023 - Omar - Arreglados tests y mas cosas
</commit_message>
<xml_diff>
--- a/docs/sdi2223-entrega1-32.xlsx
+++ b/docs/sdi2223-entrega1-32.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/delacal_uniovi_es/Documents/DOCENCIA/SDI/2223/_prácticas-propuestas/continua/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ingenieria Informatica\Tercero\Segundo_Semestre\Sistemas Distribuidos e Internet\Practicas\SDI2223-entrega1-32\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="8_{C85CB70A-9B7B-EA48-B0A5-B50919DF1CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC178D0B-4CE6-4367-BA26-9F95D162839D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
     <sheet name="Instrucciones" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -253,7 +252,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -648,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -756,6 +755,65 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -764,87 +822,32 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1126,11 +1129,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1146,96 +1149,96 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48"/>
+      <c r="B2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="4" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="50">
+      <c r="B4" s="63">
         <f>H35</f>
-        <v>1.125</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
     </row>
     <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50">
+      <c r="B6" s="63">
         <f>H77</f>
         <v>3</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
     </row>
     <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="55">
+      <c r="B8" s="47">
         <f>B4-B6</f>
-        <v>-1.875</v>
-      </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
+        <v>-1</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
@@ -1267,27 +1270,27 @@
         <v>1</v>
       </c>
       <c r="C13" s="20">
-        <f>COUNTIF($C$82:$C$142,B13)</f>
+        <f t="shared" ref="C13:C27" si="0">COUNTIF($C$82:$C$142,B13)</f>
         <v>4</v>
       </c>
       <c r="D13" s="33">
         <v>0.25</v>
       </c>
       <c r="E13" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=OK")</f>
-        <v>2</v>
+        <f t="shared" ref="E13:E27" si="1">COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=OK")</f>
+        <v>4</v>
       </c>
       <c r="F13" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" ref="F13:F27" si="2">COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=FAIL")</f>
         <v>0</v>
       </c>
       <c r="G13" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=SIN")</f>
-        <v>2</v>
+        <f t="shared" ref="G13:G27" si="3">COUNTIFS($C$82:$C$142,$B13,$E$82:$E$142,"=SIN")</f>
+        <v>0</v>
       </c>
       <c r="H13" s="20">
         <f>MIN(D13,(E13/C12)*D13)</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -1295,27 +1298,27 @@
         <v>2</v>
       </c>
       <c r="C14" s="20">
-        <f>COUNTIF($C$82:$C$142,B14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D14" s="20">
         <v>0.25</v>
       </c>
       <c r="E14" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B14,$E$82:$E$142,"=OK")</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="F14" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B14,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B14,$E$82:$E$142,"=SIN")</f>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H14" s="20">
-        <f t="shared" ref="H14:H30" si="0">MIN(D14,(E14/C14)*D14)</f>
-        <v>0</v>
+        <f t="shared" ref="H14:H30" si="4">MIN(D14,(E14/C14)*D14)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1323,27 +1326,27 @@
         <v>3</v>
       </c>
       <c r="C15" s="20">
-        <f>COUNTIF($C$82:$C$142,B15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D15" s="20">
         <v>0.25</v>
       </c>
       <c r="E15" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B15,$E$82:$E$142,"=OK")</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="F15" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B15,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B15,$E$82:$E$142,"=SIN")</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H15" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1351,27 +1354,27 @@
         <v>4</v>
       </c>
       <c r="C16" s="20">
-        <f>COUNTIF($C$82:$C$142,B16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D16" s="20">
         <v>0.25</v>
       </c>
       <c r="E16" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B16,$E$82:$E$142,"=OK")</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="F16" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B16,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B16,$E$82:$E$142,"=SIN")</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H16" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1379,26 +1382,26 @@
         <v>5</v>
       </c>
       <c r="C17" s="20">
-        <f>COUNTIF($C$82:$C$142,B17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D17" s="20">
         <v>0.5</v>
       </c>
       <c r="E17" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B17,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F17" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B17,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B17,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H17" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1407,26 +1410,26 @@
         <v>6</v>
       </c>
       <c r="C18" s="20">
-        <f>COUNTIF($C$82:$C$142,B18)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D18" s="20">
         <v>0.5</v>
       </c>
       <c r="E18" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B18,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F18" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B18,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B18,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H18" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1435,26 +1438,26 @@
         <v>7</v>
       </c>
       <c r="C19" s="20">
-        <f>COUNTIF($C$82:$C$142,B19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D19" s="20">
         <v>0.25</v>
       </c>
       <c r="E19" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B19,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F19" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B19,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B19,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H19" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1463,26 +1466,26 @@
         <v>8</v>
       </c>
       <c r="C20" s="20">
-        <f>COUNTIF($C$82:$C$142,B20)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D20" s="20">
         <v>0.5</v>
       </c>
       <c r="E20" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B20,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F20" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B20,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B20,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H20" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1491,26 +1494,26 @@
         <v>9</v>
       </c>
       <c r="C21" s="20">
-        <f>COUNTIF($C$82:$C$142,B21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D21" s="20">
         <v>0.5</v>
       </c>
       <c r="E21" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B21,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F21" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B21,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B21,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H21" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1519,26 +1522,26 @@
         <v>10</v>
       </c>
       <c r="C22" s="20">
-        <f>COUNTIF($C$82:$C$142,B22)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D22" s="20">
         <v>0.5</v>
       </c>
       <c r="E22" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B22,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F22" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B22,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B22,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H22" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1547,26 +1550,26 @@
         <v>11</v>
       </c>
       <c r="C23" s="20">
-        <f>COUNTIF($C$82:$C$142,B23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D23" s="20">
         <v>0.5</v>
       </c>
       <c r="E23" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B23,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F23" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B23,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B23,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H23" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1575,26 +1578,26 @@
         <v>12</v>
       </c>
       <c r="C24" s="20">
-        <f>COUNTIF($C$82:$C$142,B24)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D24" s="20">
         <v>0.75</v>
       </c>
       <c r="E24" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B24,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F24" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B24,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G24" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B24,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H24" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1603,26 +1606,26 @@
         <v>13</v>
       </c>
       <c r="C25" s="20">
-        <f>COUNTIF($C$82:$C$142,B25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D25" s="20">
         <v>0.5</v>
       </c>
       <c r="E25" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B25,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B25,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B25,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H25" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1631,22 +1634,22 @@
         <v>14</v>
       </c>
       <c r="C26" s="20">
-        <f>COUNTIF($C$82:$C$142,B26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D26" s="20">
         <v>0.5</v>
       </c>
       <c r="E26" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B26,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F26" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B26,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G26" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B26,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H26" s="20">
@@ -1659,22 +1662,22 @@
         <v>15</v>
       </c>
       <c r="C27" s="20">
-        <f>COUNTIF($C$82:$C$142,B27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D27" s="20">
         <v>1</v>
       </c>
       <c r="E27" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B27,$E$82:$E$142,"=OK")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F27" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B27,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G27" s="20">
-        <f>COUNTIFS($C$82:$C$142,$B27,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H27" s="20">
@@ -1695,7 +1698,7 @@
       </c>
       <c r="E28" s="9">
         <f>COUNTIFS($C$82:$C$129,$B28,$E$82:$E$129,"=OK")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="9">
         <f>COUNTIFS($C$82:$C$129,$B28,$E$82:$E$129,"FAIL")</f>
@@ -1703,7 +1706,7 @@
       </c>
       <c r="G28" s="9">
         <f>COUNTIFS($C$82:$C$129,$B28,$E$82:$E$129,"=SIN")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="38">
         <v>1</v>
@@ -1721,7 +1724,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="34">
         <f>SUM(H13:H28)</f>
-        <v>1.125</v>
+        <v>2</v>
       </c>
       <c r="I29" s="35" t="s">
         <v>12</v>
@@ -1732,26 +1735,26 @@
         <v>17</v>
       </c>
       <c r="C30" s="20">
-        <f t="shared" ref="C30:C31" si="1">COUNTIF($C$82:$C$142,B30)</f>
+        <f t="shared" ref="C30:C31" si="5">COUNTIF($C$82:$C$142,B30)</f>
         <v>2</v>
       </c>
       <c r="D30" s="20">
         <v>0.5</v>
       </c>
       <c r="E30" s="20">
-        <f t="shared" ref="E30:E33" si="2">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=OK")</f>
+        <f t="shared" ref="E30:E33" si="6">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=OK")</f>
         <v>0</v>
       </c>
       <c r="F30" s="20">
-        <f t="shared" ref="F30:F33" si="3">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=FAIL")</f>
+        <f t="shared" ref="F30:F33" si="7">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=FAIL")</f>
         <v>0</v>
       </c>
       <c r="G30" s="20">
-        <f t="shared" ref="G30:G33" si="4">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=SIN")</f>
+        <f t="shared" ref="G30:G32" si="8">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=SIN")</f>
         <v>2</v>
       </c>
-      <c r="H30" s="67">
-        <f t="shared" si="0"/>
+      <c r="H30" s="42">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1760,22 +1763,22 @@
         <v>18</v>
       </c>
       <c r="C31" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D31" s="20">
         <v>1</v>
       </c>
       <c r="E31" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F31" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G31" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H31" s="20">
@@ -1795,15 +1798,15 @@
         <v>1.5</v>
       </c>
       <c r="E32" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F32" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G32" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H32" s="20">
@@ -1821,11 +1824,11 @@
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F33" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G33" s="20">
@@ -1833,7 +1836,7 @@
         <v>4</v>
       </c>
       <c r="H33" s="20">
-        <f t="shared" ref="H33" si="5">MIN(D33,(E33/C33)*D33)</f>
+        <f t="shared" ref="H33" si="9">MIN(D33,(E33/C33)*D33)</f>
         <v>0</v>
       </c>
     </row>
@@ -1866,22 +1869,22 @@
       <c r="G35" s="37"/>
       <c r="H35" s="22">
         <f>H29+H34</f>
-        <v>1.125</v>
+        <v>2</v>
       </c>
       <c r="I35" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="58"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="39"/>
       <c r="J36" s="38" t="s">
         <v>17</v>
@@ -1891,13 +1894,13 @@
       <c r="B37" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="24" t="s">
         <v>20</v>
       </c>
@@ -1912,13 +1915,13 @@
       <c r="B38" s="25">
         <v>1</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
       <c r="H38" s="16">
         <f>J38</f>
         <v>1</v>
@@ -1934,15 +1937,15 @@
       <c r="B39" s="25">
         <v>2</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
       <c r="H39" s="16">
-        <f t="shared" ref="H39:H40" si="6">J39</f>
+        <f t="shared" ref="H39:H40" si="10">J39</f>
         <v>1</v>
       </c>
       <c r="I39" s="13">
@@ -1956,15 +1959,15 @@
       <c r="B40" s="25">
         <v>3</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
       <c r="H40" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I40" s="13">
@@ -1978,11 +1981,11 @@
       <c r="B41" s="25">
         <v>4</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
       <c r="H41" s="16"/>
       <c r="I41" s="13"/>
       <c r="J41" s="17"/>
@@ -1991,11 +1994,11 @@
       <c r="B42" s="25">
         <v>5</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
       <c r="H42" s="16"/>
       <c r="I42" s="13"/>
       <c r="J42" s="17"/>
@@ -2004,11 +2007,11 @@
       <c r="B43" s="25">
         <v>6</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
       <c r="H43" s="16"/>
       <c r="I43" s="13"/>
       <c r="J43" s="17"/>
@@ -2017,11 +2020,11 @@
       <c r="B44" s="25">
         <v>7</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
       <c r="H44" s="16"/>
       <c r="I44" s="13"/>
       <c r="J44" s="17"/>
@@ -2030,11 +2033,11 @@
       <c r="B45" s="25">
         <v>8</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
       <c r="H45" s="16"/>
       <c r="I45" s="13"/>
       <c r="J45" s="17"/>
@@ -2043,11 +2046,11 @@
       <c r="B46" s="25">
         <v>9</v>
       </c>
-      <c r="C46" s="41"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
       <c r="H46" s="16"/>
       <c r="I46" s="13"/>
       <c r="J46" s="17"/>
@@ -2056,11 +2059,11 @@
       <c r="B47" s="25">
         <v>10</v>
       </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="16"/>
       <c r="I47" s="13"/>
       <c r="J47" s="17"/>
@@ -2069,11 +2072,11 @@
       <c r="B48" s="25">
         <v>11</v>
       </c>
-      <c r="C48" s="41"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
       <c r="H48" s="16"/>
       <c r="I48" s="13"/>
       <c r="J48" s="17"/>
@@ -2082,11 +2085,11 @@
       <c r="B49" s="25">
         <v>12</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="16"/>
       <c r="I49" s="13"/>
       <c r="J49" s="17"/>
@@ -2095,11 +2098,11 @@
       <c r="B50" s="25">
         <v>13</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
       <c r="H50" s="16"/>
       <c r="I50" s="13"/>
       <c r="J50" s="17"/>
@@ -2108,11 +2111,11 @@
       <c r="B51" s="25">
         <v>14</v>
       </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
       <c r="H51" s="16"/>
       <c r="I51" s="13"/>
       <c r="J51" s="17"/>
@@ -2121,11 +2124,11 @@
       <c r="B52" s="25">
         <v>15</v>
       </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
       <c r="H52" s="16"/>
       <c r="I52" s="13"/>
       <c r="J52" s="17"/>
@@ -2134,11 +2137,11 @@
       <c r="B53" s="25">
         <v>16</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
       <c r="H53" s="16"/>
       <c r="I53" s="13"/>
       <c r="J53" s="17"/>
@@ -2147,11 +2150,11 @@
       <c r="B54" s="25">
         <v>17</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
       <c r="H54" s="16"/>
       <c r="I54" s="13"/>
       <c r="J54" s="17"/>
@@ -2160,11 +2163,11 @@
       <c r="B55" s="25">
         <v>18</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
       <c r="H55" s="16"/>
       <c r="I55" s="13"/>
       <c r="J55" s="17"/>
@@ -2173,11 +2176,11 @@
       <c r="B56" s="25">
         <v>19</v>
       </c>
-      <c r="C56" s="41"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
       <c r="H56" s="16"/>
       <c r="I56" s="13"/>
       <c r="J56" s="17"/>
@@ -2186,11 +2189,11 @@
       <c r="B57" s="25">
         <v>20</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
       <c r="H57" s="16"/>
       <c r="I57" s="13"/>
       <c r="J57" s="17"/>
@@ -2199,11 +2202,11 @@
       <c r="B58" s="25">
         <v>21</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
       <c r="H58" s="16"/>
       <c r="I58" s="13"/>
       <c r="J58" s="17"/>
@@ -2212,11 +2215,11 @@
       <c r="B59" s="25">
         <v>22</v>
       </c>
-      <c r="C59" s="41"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
       <c r="H59" s="16"/>
       <c r="I59" s="13"/>
       <c r="J59" s="17"/>
@@ -2225,11 +2228,11 @@
       <c r="B60" s="25">
         <v>23</v>
       </c>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="60"/>
+      <c r="F60" s="60"/>
+      <c r="G60" s="60"/>
       <c r="H60" s="16"/>
       <c r="I60" s="13"/>
       <c r="J60" s="17"/>
@@ -2238,11 +2241,11 @@
       <c r="B61" s="25">
         <v>24</v>
       </c>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
       <c r="H61" s="16"/>
       <c r="I61" s="13"/>
       <c r="J61" s="17"/>
@@ -2251,11 +2254,11 @@
       <c r="B62" s="25">
         <v>25</v>
       </c>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="60"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="60"/>
       <c r="H62" s="16"/>
       <c r="I62" s="13"/>
       <c r="J62" s="17"/>
@@ -2264,11 +2267,11 @@
       <c r="B63" s="25">
         <v>26</v>
       </c>
-      <c r="C63" s="41"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="60"/>
       <c r="H63" s="16"/>
       <c r="I63" s="13"/>
       <c r="J63" s="17"/>
@@ -2277,11 +2280,11 @@
       <c r="B64" s="25">
         <v>27</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="60"/>
+      <c r="G64" s="60"/>
       <c r="H64" s="16"/>
       <c r="I64" s="13"/>
       <c r="J64" s="17"/>
@@ -2290,11 +2293,11 @@
       <c r="B65" s="25">
         <v>28</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="60"/>
       <c r="H65" s="16"/>
       <c r="I65" s="13"/>
       <c r="J65" s="17"/>
@@ -2303,11 +2306,11 @@
       <c r="B66" s="25">
         <v>29</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
       <c r="H66" s="16"/>
       <c r="I66" s="13"/>
       <c r="J66" s="17"/>
@@ -2316,11 +2319,11 @@
       <c r="B67" s="25">
         <v>30</v>
       </c>
-      <c r="C67" s="41"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="60"/>
+      <c r="F67" s="60"/>
+      <c r="G67" s="60"/>
       <c r="H67" s="16"/>
       <c r="I67" s="13"/>
       <c r="J67" s="17"/>
@@ -2329,11 +2332,11 @@
       <c r="B68" s="31">
         <v>31</v>
       </c>
-      <c r="C68" s="41"/>
-      <c r="D68" s="52"/>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="65"/>
+      <c r="G68" s="65"/>
       <c r="H68" s="16"/>
       <c r="I68" s="13"/>
       <c r="J68" s="17"/>
@@ -2342,11 +2345,11 @@
       <c r="B69" s="31">
         <v>32</v>
       </c>
-      <c r="C69" s="41"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="52"/>
-      <c r="F69" s="52"/>
-      <c r="G69" s="52"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="65"/>
+      <c r="E69" s="65"/>
+      <c r="F69" s="65"/>
+      <c r="G69" s="65"/>
       <c r="H69" s="16"/>
       <c r="I69" s="13"/>
       <c r="J69" s="17"/>
@@ -2355,11 +2358,11 @@
       <c r="B70" s="31">
         <v>33</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="52"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="52"/>
-      <c r="G70" s="52"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="65"/>
+      <c r="F70" s="65"/>
+      <c r="G70" s="65"/>
       <c r="H70" s="16"/>
       <c r="I70" s="13"/>
       <c r="J70" s="17"/>
@@ -2368,11 +2371,11 @@
       <c r="B71" s="31">
         <v>34</v>
       </c>
-      <c r="C71" s="53"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="67"/>
+      <c r="F71" s="67"/>
+      <c r="G71" s="67"/>
       <c r="H71" s="40"/>
       <c r="I71" s="13"/>
       <c r="J71" s="17"/>
@@ -2381,11 +2384,11 @@
       <c r="B72" s="20">
         <v>35</v>
       </c>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
-      <c r="G72" s="51"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
       <c r="H72" s="36"/>
       <c r="I72" s="13"/>
       <c r="J72" s="17"/>
@@ -2394,11 +2397,11 @@
       <c r="B73" s="20">
         <v>36</v>
       </c>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
-      <c r="F73" s="51"/>
-      <c r="G73" s="51"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
       <c r="H73" s="36"/>
       <c r="I73" s="13"/>
       <c r="J73" s="17"/>
@@ -2407,11 +2410,11 @@
       <c r="B74" s="20">
         <v>38</v>
       </c>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
-      <c r="G74" s="51"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="64"/>
       <c r="H74" s="36"/>
       <c r="I74" s="13"/>
       <c r="J74" s="17"/>
@@ -2420,11 +2423,11 @@
       <c r="B75" s="20">
         <v>39</v>
       </c>
-      <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="51"/>
-      <c r="F75" s="51"/>
-      <c r="G75" s="51"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
       <c r="H75" s="36"/>
       <c r="I75" s="13"/>
       <c r="J75" s="17"/>
@@ -2433,11 +2436,11 @@
       <c r="B76" s="26">
         <v>40</v>
       </c>
-      <c r="C76" s="51"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="51"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="64"/>
       <c r="H76" s="36"/>
       <c r="I76" s="13"/>
       <c r="J76" s="17"/>
@@ -2478,15 +2481,15 @@
       <c r="H79" s="20"/>
     </row>
     <row r="80" spans="2:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B80" s="59" t="s">
+      <c r="B80" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="60"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="60"/>
-      <c r="F80" s="60"/>
-      <c r="G80" s="60"/>
-      <c r="H80" s="61"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="55"/>
+      <c r="G80" s="55"/>
+      <c r="H80" s="56"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
@@ -2501,11 +2504,11 @@
       <c r="E81" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F81" s="44" t="s">
+      <c r="F81" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
       <c r="J81" s="32"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -2553,7 +2556,7 @@
         <v>33</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F84" s="43"/>
       <c r="G84" s="43"/>
@@ -2569,8 +2572,8 @@
       <c r="D85" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E85" s="14" t="s">
-        <v>34</v>
+      <c r="E85" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F85" s="43"/>
       <c r="G85" s="43"/>
@@ -2586,8 +2589,8 @@
       <c r="D86" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E86" s="14" t="s">
-        <v>34</v>
+      <c r="E86" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F86" s="43"/>
       <c r="G86" s="43"/>
@@ -2603,8 +2606,8 @@
       <c r="D87" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E87" s="14" t="s">
-        <v>34</v>
+      <c r="E87" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F87" s="43"/>
       <c r="G87" s="43"/>
@@ -2620,8 +2623,8 @@
       <c r="D88" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E88" s="14" t="s">
-        <v>34</v>
+      <c r="E88" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F88" s="43"/>
       <c r="G88" s="43"/>
@@ -2637,8 +2640,8 @@
       <c r="D89" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E89" s="14" t="s">
-        <v>34</v>
+      <c r="E89" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F89" s="43"/>
       <c r="G89" s="43"/>
@@ -2654,8 +2657,8 @@
       <c r="D90" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E90" s="14" t="s">
-        <v>34</v>
+      <c r="E90" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F90" s="43"/>
       <c r="G90" s="43"/>
@@ -2671,8 +2674,8 @@
       <c r="D91" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E91" s="14" t="s">
-        <v>34</v>
+      <c r="E91" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F91" s="43"/>
       <c r="G91" s="43"/>
@@ -2688,8 +2691,8 @@
       <c r="D92" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E92" s="14" t="s">
-        <v>34</v>
+      <c r="E92" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="F92" s="43"/>
       <c r="G92" s="43"/>
@@ -3097,7 +3100,7 @@
         <v>33</v>
       </c>
       <c r="E116" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F116" s="43"/>
       <c r="G116" s="43"/>
@@ -3133,9 +3136,9 @@
       <c r="E118" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F118" s="64"/>
-      <c r="G118" s="65"/>
-      <c r="H118" s="66"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="45"/>
+      <c r="H118" s="46"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B119" s="20">
@@ -3150,9 +3153,9 @@
       <c r="E119" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F119" s="64"/>
-      <c r="G119" s="65"/>
-      <c r="H119" s="66"/>
+      <c r="F119" s="44"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="46"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B120" s="20">
@@ -3167,9 +3170,9 @@
       <c r="E120" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F120" s="64"/>
-      <c r="G120" s="65"/>
-      <c r="H120" s="66"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="45"/>
+      <c r="H120" s="46"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B121" s="20">
@@ -3551,46 +3554,54 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="lCPgoHp4bLbIL1JNSK1ttH4+ZWvchbvc6Q2GSYOJu0YqXyyM/lw16pZxohXMjvCxn31f3hDIG8XQ3rUZmvOdDA==" saltValue="q8lea4feKY9l39UvYwa3nA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="112">
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C67:G67"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C68:G68"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C61:G61"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="B36:H36"/>
@@ -3615,67 +3626,59 @@
     <mergeCell ref="C63:G63"/>
     <mergeCell ref="C64:G64"/>
     <mergeCell ref="C65:G65"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="C67:G67"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Instrucciones!$A$7:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>D82:D142</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{9AD118CD-499E-1142-9514-76C61E9D8D60}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Instrucciones!$A$13:$A$15</xm:f>
           </x14:formula1>
@@ -3688,7 +3691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
19/03/2023 - Omar - Ultimo commit (espero)
</commit_message>
<xml_diff>
--- a/docs/sdi2223-entrega1-32.xlsx
+++ b/docs/sdi2223-entrega1-32.xlsx
@@ -755,17 +755,89 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -777,78 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1160,73 +1160,73 @@
       <c r="H2" s="50"/>
     </row>
     <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="63">
+      <c r="B4" s="52">
         <f>H35</f>
+        <v>11</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+    </row>
+    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-    </row>
-    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="63">
+      <c r="B6" s="52">
         <f>H77</f>
         <v>3</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
     </row>
     <row r="7" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="47">
+      <c r="B8" s="57">
         <f>B4-B6</f>
-        <v>-1</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="E17" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="20">
         <f t="shared" si="2"/>
@@ -1398,11 +1398,11 @@
       </c>
       <c r="G17" s="20">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E18" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="20">
         <f t="shared" si="2"/>
@@ -1426,11 +1426,11 @@
       </c>
       <c r="G18" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="E19" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="20">
         <f t="shared" si="2"/>
@@ -1454,11 +1454,11 @@
       </c>
       <c r="G19" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E20" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="20">
         <f t="shared" si="2"/>
@@ -1482,11 +1482,11 @@
       </c>
       <c r="G20" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H20" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E21" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="20">
         <f t="shared" si="2"/>
@@ -1510,11 +1510,11 @@
       </c>
       <c r="G21" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="E22" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22" s="20">
         <f t="shared" si="2"/>
@@ -1538,11 +1538,11 @@
       </c>
       <c r="G22" s="20">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="E23" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="20">
         <f t="shared" si="2"/>
@@ -1566,11 +1566,11 @@
       </c>
       <c r="G23" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="E24" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" s="20">
         <f t="shared" si="2"/>
@@ -1594,11 +1594,11 @@
       </c>
       <c r="G24" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H24" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="E25" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="20">
         <f t="shared" si="2"/>
@@ -1622,11 +1622,11 @@
       </c>
       <c r="G25" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="E26" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="20">
         <f t="shared" si="2"/>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="G26" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="20">
         <f>MIN(D26,(E26/C26)*D26)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="E27" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F27" s="20">
         <f t="shared" si="2"/>
@@ -1678,11 +1678,11 @@
       </c>
       <c r="G27" s="20">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="20">
         <f>MIN(D27,(E27/C27)*D27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="34">
         <f>SUM(H13:H28)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I29" s="35" t="s">
         <v>12</v>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="E30" s="20">
         <f t="shared" ref="E30:E33" si="6">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=OK")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="20">
         <f t="shared" ref="F30:F33" si="7">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=FAIL")</f>
@@ -1751,11 +1751,11 @@
       </c>
       <c r="G30" s="20">
         <f t="shared" ref="G30:G32" si="8">COUNTIFS($C$82:$C$142,$B30,$E$82:$E$142,"=SIN")</f>
-        <v>2</v>
-      </c>
-      <c r="H30" s="42">
+        <v>0</v>
+      </c>
+      <c r="H30" s="41">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="E31" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="20">
         <f t="shared" si="7"/>
@@ -1779,11 +1779,11 @@
       </c>
       <c r="G31" s="20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H31" s="20">
         <f>MIN(D31,(E31/C31)*D31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="E32" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="7"/>
@@ -1807,11 +1807,11 @@
       </c>
       <c r="G32" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H32" s="20">
         <f>MIN(D32,(E32/C32)*D32)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
       <c r="G34" s="20"/>
       <c r="H34" s="22">
         <f>SUM(H30:H33)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I34" s="35" t="s">
         <v>13</v>
@@ -1869,22 +1869,22 @@
       <c r="G35" s="37"/>
       <c r="H35" s="22">
         <f>H29+H34</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I35" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="53"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="60"/>
       <c r="I36" s="39"/>
       <c r="J36" s="38" t="s">
         <v>17</v>
@@ -1894,13 +1894,13 @@
       <c r="B37" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
       <c r="H37" s="24" t="s">
         <v>20</v>
       </c>
@@ -1915,13 +1915,13 @@
       <c r="B38" s="25">
         <v>1</v>
       </c>
-      <c r="C38" s="59" t="s">
+      <c r="C38" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="16">
         <f>J38</f>
         <v>1</v>
@@ -1937,13 +1937,13 @@
       <c r="B39" s="25">
         <v>2</v>
       </c>
-      <c r="C39" s="59" t="s">
+      <c r="C39" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
       <c r="H39" s="16">
         <f t="shared" ref="H39:H40" si="10">J39</f>
         <v>1</v>
@@ -1959,13 +1959,13 @@
       <c r="B40" s="25">
         <v>3</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="16">
         <f t="shared" si="10"/>
         <v>1</v>
@@ -1981,11 +1981,11 @@
       <c r="B41" s="25">
         <v>4</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
       <c r="H41" s="16"/>
       <c r="I41" s="13"/>
       <c r="J41" s="17"/>
@@ -1994,11 +1994,11 @@
       <c r="B42" s="25">
         <v>5</v>
       </c>
-      <c r="C42" s="59"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
       <c r="H42" s="16"/>
       <c r="I42" s="13"/>
       <c r="J42" s="17"/>
@@ -2007,11 +2007,11 @@
       <c r="B43" s="25">
         <v>6</v>
       </c>
-      <c r="C43" s="59"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
       <c r="H43" s="16"/>
       <c r="I43" s="13"/>
       <c r="J43" s="17"/>
@@ -2020,11 +2020,11 @@
       <c r="B44" s="25">
         <v>7</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
       <c r="H44" s="16"/>
       <c r="I44" s="13"/>
       <c r="J44" s="17"/>
@@ -2033,11 +2033,11 @@
       <c r="B45" s="25">
         <v>8</v>
       </c>
-      <c r="C45" s="59"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
       <c r="H45" s="16"/>
       <c r="I45" s="13"/>
       <c r="J45" s="17"/>
@@ -2046,11 +2046,11 @@
       <c r="B46" s="25">
         <v>9</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
       <c r="H46" s="16"/>
       <c r="I46" s="13"/>
       <c r="J46" s="17"/>
@@ -2059,11 +2059,11 @@
       <c r="B47" s="25">
         <v>10</v>
       </c>
-      <c r="C47" s="59"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
       <c r="H47" s="16"/>
       <c r="I47" s="13"/>
       <c r="J47" s="17"/>
@@ -2072,11 +2072,11 @@
       <c r="B48" s="25">
         <v>11</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="60"/>
-      <c r="G48" s="60"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
       <c r="H48" s="16"/>
       <c r="I48" s="13"/>
       <c r="J48" s="17"/>
@@ -2085,11 +2085,11 @@
       <c r="B49" s="25">
         <v>12</v>
       </c>
-      <c r="C49" s="59"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
       <c r="H49" s="16"/>
       <c r="I49" s="13"/>
       <c r="J49" s="17"/>
@@ -2098,11 +2098,11 @@
       <c r="B50" s="25">
         <v>13</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
       <c r="H50" s="16"/>
       <c r="I50" s="13"/>
       <c r="J50" s="17"/>
@@ -2111,11 +2111,11 @@
       <c r="B51" s="25">
         <v>14</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
       <c r="H51" s="16"/>
       <c r="I51" s="13"/>
       <c r="J51" s="17"/>
@@ -2124,11 +2124,11 @@
       <c r="B52" s="25">
         <v>15</v>
       </c>
-      <c r="C52" s="59"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60"/>
-      <c r="G52" s="60"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
       <c r="H52" s="16"/>
       <c r="I52" s="13"/>
       <c r="J52" s="17"/>
@@ -2137,11 +2137,11 @@
       <c r="B53" s="25">
         <v>16</v>
       </c>
-      <c r="C53" s="59"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
       <c r="H53" s="16"/>
       <c r="I53" s="13"/>
       <c r="J53" s="17"/>
@@ -2150,11 +2150,11 @@
       <c r="B54" s="25">
         <v>17</v>
       </c>
-      <c r="C54" s="59"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="60"/>
-      <c r="F54" s="60"/>
-      <c r="G54" s="60"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
       <c r="H54" s="16"/>
       <c r="I54" s="13"/>
       <c r="J54" s="17"/>
@@ -2163,11 +2163,11 @@
       <c r="B55" s="25">
         <v>18</v>
       </c>
-      <c r="C55" s="59"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
       <c r="H55" s="16"/>
       <c r="I55" s="13"/>
       <c r="J55" s="17"/>
@@ -2176,11 +2176,11 @@
       <c r="B56" s="25">
         <v>19</v>
       </c>
-      <c r="C56" s="59"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="60"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
       <c r="H56" s="16"/>
       <c r="I56" s="13"/>
       <c r="J56" s="17"/>
@@ -2189,11 +2189,11 @@
       <c r="B57" s="25">
         <v>20</v>
       </c>
-      <c r="C57" s="59"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
       <c r="H57" s="16"/>
       <c r="I57" s="13"/>
       <c r="J57" s="17"/>
@@ -2202,11 +2202,11 @@
       <c r="B58" s="25">
         <v>21</v>
       </c>
-      <c r="C58" s="59"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="60"/>
-      <c r="F58" s="60"/>
-      <c r="G58" s="60"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
       <c r="H58" s="16"/>
       <c r="I58" s="13"/>
       <c r="J58" s="17"/>
@@ -2215,11 +2215,11 @@
       <c r="B59" s="25">
         <v>22</v>
       </c>
-      <c r="C59" s="59"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
       <c r="H59" s="16"/>
       <c r="I59" s="13"/>
       <c r="J59" s="17"/>
@@ -2228,11 +2228,11 @@
       <c r="B60" s="25">
         <v>23</v>
       </c>
-      <c r="C60" s="59"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="60"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="60"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
       <c r="H60" s="16"/>
       <c r="I60" s="13"/>
       <c r="J60" s="17"/>
@@ -2241,11 +2241,11 @@
       <c r="B61" s="25">
         <v>24</v>
       </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
       <c r="H61" s="16"/>
       <c r="I61" s="13"/>
       <c r="J61" s="17"/>
@@ -2254,11 +2254,11 @@
       <c r="B62" s="25">
         <v>25</v>
       </c>
-      <c r="C62" s="59"/>
-      <c r="D62" s="60"/>
-      <c r="E62" s="60"/>
-      <c r="F62" s="60"/>
-      <c r="G62" s="60"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
       <c r="H62" s="16"/>
       <c r="I62" s="13"/>
       <c r="J62" s="17"/>
@@ -2267,11 +2267,11 @@
       <c r="B63" s="25">
         <v>26</v>
       </c>
-      <c r="C63" s="59"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="60"/>
-      <c r="G63" s="60"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
       <c r="H63" s="16"/>
       <c r="I63" s="13"/>
       <c r="J63" s="17"/>
@@ -2280,11 +2280,11 @@
       <c r="B64" s="25">
         <v>27</v>
       </c>
-      <c r="C64" s="59"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
       <c r="H64" s="16"/>
       <c r="I64" s="13"/>
       <c r="J64" s="17"/>
@@ -2293,11 +2293,11 @@
       <c r="B65" s="25">
         <v>28</v>
       </c>
-      <c r="C65" s="59"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
       <c r="H65" s="16"/>
       <c r="I65" s="13"/>
       <c r="J65" s="17"/>
@@ -2306,11 +2306,11 @@
       <c r="B66" s="25">
         <v>29</v>
       </c>
-      <c r="C66" s="59"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
       <c r="H66" s="16"/>
       <c r="I66" s="13"/>
       <c r="J66" s="17"/>
@@ -2319,11 +2319,11 @@
       <c r="B67" s="25">
         <v>30</v>
       </c>
-      <c r="C67" s="59"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
       <c r="H67" s="16"/>
       <c r="I67" s="13"/>
       <c r="J67" s="17"/>
@@ -2332,11 +2332,11 @@
       <c r="B68" s="31">
         <v>31</v>
       </c>
-      <c r="C68" s="59"/>
-      <c r="D68" s="65"/>
-      <c r="E68" s="65"/>
-      <c r="F68" s="65"/>
-      <c r="G68" s="65"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="54"/>
       <c r="H68" s="16"/>
       <c r="I68" s="13"/>
       <c r="J68" s="17"/>
@@ -2345,11 +2345,11 @@
       <c r="B69" s="31">
         <v>32</v>
       </c>
-      <c r="C69" s="59"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="16"/>
       <c r="I69" s="13"/>
       <c r="J69" s="17"/>
@@ -2358,11 +2358,11 @@
       <c r="B70" s="31">
         <v>33</v>
       </c>
-      <c r="C70" s="59"/>
-      <c r="D70" s="65"/>
-      <c r="E70" s="65"/>
-      <c r="F70" s="65"/>
-      <c r="G70" s="65"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="54"/>
       <c r="H70" s="16"/>
       <c r="I70" s="13"/>
       <c r="J70" s="17"/>
@@ -2371,11 +2371,11 @@
       <c r="B71" s="31">
         <v>34</v>
       </c>
-      <c r="C71" s="66"/>
-      <c r="D71" s="67"/>
-      <c r="E71" s="67"/>
-      <c r="F71" s="67"/>
-      <c r="G71" s="67"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
+      <c r="G71" s="56"/>
       <c r="H71" s="40"/>
       <c r="I71" s="13"/>
       <c r="J71" s="17"/>
@@ -2384,11 +2384,11 @@
       <c r="B72" s="20">
         <v>35</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
       <c r="H72" s="36"/>
       <c r="I72" s="13"/>
       <c r="J72" s="17"/>
@@ -2397,11 +2397,11 @@
       <c r="B73" s="20">
         <v>36</v>
       </c>
-      <c r="C73" s="64"/>
-      <c r="D73" s="64"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="64"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
       <c r="H73" s="36"/>
       <c r="I73" s="13"/>
       <c r="J73" s="17"/>
@@ -2410,11 +2410,11 @@
       <c r="B74" s="20">
         <v>38</v>
       </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="64"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="53"/>
+      <c r="E74" s="53"/>
+      <c r="F74" s="53"/>
+      <c r="G74" s="53"/>
       <c r="H74" s="36"/>
       <c r="I74" s="13"/>
       <c r="J74" s="17"/>
@@ -2423,11 +2423,11 @@
       <c r="B75" s="20">
         <v>39</v>
       </c>
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
       <c r="H75" s="36"/>
       <c r="I75" s="13"/>
       <c r="J75" s="17"/>
@@ -2436,11 +2436,11 @@
       <c r="B76" s="26">
         <v>40</v>
       </c>
-      <c r="C76" s="64"/>
-      <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
-      <c r="F76" s="64"/>
-      <c r="G76" s="64"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
       <c r="H76" s="36"/>
       <c r="I76" s="13"/>
       <c r="J76" s="17"/>
@@ -2481,15 +2481,15 @@
       <c r="H79" s="20"/>
     </row>
     <row r="80" spans="2:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B80" s="54" t="s">
+      <c r="B80" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="55"/>
-      <c r="D80" s="55"/>
-      <c r="E80" s="55"/>
-      <c r="F80" s="55"/>
-      <c r="G80" s="55"/>
-      <c r="H80" s="56"/>
+      <c r="C80" s="62"/>
+      <c r="D80" s="62"/>
+      <c r="E80" s="62"/>
+      <c r="F80" s="62"/>
+      <c r="G80" s="62"/>
+      <c r="H80" s="63"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
@@ -2504,11 +2504,11 @@
       <c r="E81" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F81" s="68" t="s">
+      <c r="F81" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
+      <c r="G81" s="46"/>
+      <c r="H81" s="46"/>
       <c r="J81" s="32"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -2521,12 +2521,12 @@
       <c r="D82" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F82" s="43"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="43"/>
+      <c r="E82" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="20">
@@ -2541,9 +2541,9 @@
       <c r="E83" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="45"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84" s="20">
@@ -2555,12 +2555,12 @@
       <c r="D84" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E84" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="43"/>
+      <c r="E84" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F84" s="45"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="45"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" s="20">
@@ -2572,12 +2572,12 @@
       <c r="D85" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E85" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
+      <c r="E85" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F85" s="45"/>
+      <c r="G85" s="45"/>
+      <c r="H85" s="45"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" s="20">
@@ -2589,12 +2589,12 @@
       <c r="D86" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E86" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F86" s="43"/>
-      <c r="G86" s="43"/>
-      <c r="H86" s="43"/>
+      <c r="E86" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87" s="20">
@@ -2606,12 +2606,12 @@
       <c r="D87" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E87" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F87" s="43"/>
-      <c r="G87" s="43"/>
-      <c r="H87" s="43"/>
+      <c r="E87" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88" s="20">
@@ -2623,12 +2623,12 @@
       <c r="D88" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E88" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F88" s="43"/>
-      <c r="G88" s="43"/>
-      <c r="H88" s="43"/>
+      <c r="E88" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="45"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89" s="20">
@@ -2640,12 +2640,12 @@
       <c r="D89" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E89" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F89" s="43"/>
-      <c r="G89" s="43"/>
-      <c r="H89" s="43"/>
+      <c r="E89" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" s="45"/>
+      <c r="G89" s="45"/>
+      <c r="H89" s="45"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90" s="20">
@@ -2657,12 +2657,12 @@
       <c r="D90" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E90" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F90" s="43"/>
-      <c r="G90" s="43"/>
-      <c r="H90" s="43"/>
+      <c r="E90" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F90" s="45"/>
+      <c r="G90" s="45"/>
+      <c r="H90" s="45"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91" s="20">
@@ -2674,12 +2674,12 @@
       <c r="D91" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E91" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F91" s="43"/>
-      <c r="G91" s="43"/>
-      <c r="H91" s="43"/>
+      <c r="E91" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F91" s="45"/>
+      <c r="G91" s="45"/>
+      <c r="H91" s="45"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="20">
@@ -2691,12 +2691,12 @@
       <c r="D92" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E92" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="43"/>
-      <c r="G92" s="43"/>
-      <c r="H92" s="43"/>
+      <c r="E92" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F92" s="45"/>
+      <c r="G92" s="45"/>
+      <c r="H92" s="45"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93" s="20">
@@ -2708,12 +2708,12 @@
       <c r="D93" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E93" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F93" s="43"/>
-      <c r="G93" s="43"/>
-      <c r="H93" s="43"/>
+      <c r="E93" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93" s="45"/>
+      <c r="G93" s="45"/>
+      <c r="H93" s="45"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94" s="20">
@@ -2725,12 +2725,12 @@
       <c r="D94" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E94" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F94" s="43"/>
-      <c r="G94" s="43"/>
-      <c r="H94" s="43"/>
+      <c r="E94" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F94" s="45"/>
+      <c r="G94" s="45"/>
+      <c r="H94" s="45"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" s="20">
@@ -2742,12 +2742,12 @@
       <c r="D95" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E95" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F95" s="43"/>
-      <c r="G95" s="43"/>
-      <c r="H95" s="43"/>
+      <c r="E95" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F95" s="45"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="45"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="20">
@@ -2759,12 +2759,12 @@
       <c r="D96" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E96" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F96" s="43"/>
-      <c r="G96" s="43"/>
-      <c r="H96" s="43"/>
+      <c r="E96" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F96" s="45"/>
+      <c r="G96" s="45"/>
+      <c r="H96" s="45"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="20">
@@ -2776,12 +2776,12 @@
       <c r="D97" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E97" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F97" s="43"/>
-      <c r="G97" s="43"/>
-      <c r="H97" s="43"/>
+      <c r="E97" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F97" s="45"/>
+      <c r="G97" s="45"/>
+      <c r="H97" s="45"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="20">
@@ -2793,12 +2793,12 @@
       <c r="D98" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E98" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F98" s="43"/>
-      <c r="G98" s="43"/>
-      <c r="H98" s="43"/>
+      <c r="E98" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F98" s="45"/>
+      <c r="G98" s="45"/>
+      <c r="H98" s="45"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="20">
@@ -2810,12 +2810,12 @@
       <c r="D99" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E99" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F99" s="43"/>
-      <c r="G99" s="43"/>
-      <c r="H99" s="43"/>
+      <c r="E99" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F99" s="45"/>
+      <c r="G99" s="45"/>
+      <c r="H99" s="45"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="20">
@@ -2827,12 +2827,12 @@
       <c r="D100" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E100" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F100" s="43"/>
-      <c r="G100" s="43"/>
-      <c r="H100" s="43"/>
+      <c r="E100" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F100" s="45"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="45"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="20">
@@ -2844,12 +2844,12 @@
       <c r="D101" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E101" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F101" s="43"/>
-      <c r="G101" s="43"/>
-      <c r="H101" s="43"/>
+      <c r="E101" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F101" s="45"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="45"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="20">
@@ -2861,12 +2861,12 @@
       <c r="D102" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E102" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F102" s="43"/>
-      <c r="G102" s="43"/>
-      <c r="H102" s="43"/>
+      <c r="E102" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F102" s="45"/>
+      <c r="G102" s="45"/>
+      <c r="H102" s="45"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="20">
@@ -2878,12 +2878,12 @@
       <c r="D103" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F103" s="43"/>
-      <c r="G103" s="43"/>
-      <c r="H103" s="43"/>
+      <c r="E103" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F103" s="45"/>
+      <c r="G103" s="45"/>
+      <c r="H103" s="45"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="20">
@@ -2895,12 +2895,12 @@
       <c r="D104" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E104" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F104" s="43"/>
-      <c r="G104" s="43"/>
-      <c r="H104" s="43"/>
+      <c r="E104" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F104" s="45"/>
+      <c r="G104" s="45"/>
+      <c r="H104" s="45"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="20">
@@ -2912,12 +2912,12 @@
       <c r="D105" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E105" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F105" s="43"/>
-      <c r="G105" s="43"/>
-      <c r="H105" s="43"/>
+      <c r="E105" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F105" s="45"/>
+      <c r="G105" s="45"/>
+      <c r="H105" s="45"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="20">
@@ -2929,12 +2929,12 @@
       <c r="D106" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E106" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F106" s="43"/>
-      <c r="G106" s="43"/>
-      <c r="H106" s="43"/>
+      <c r="E106" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" s="45"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="45"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="20">
@@ -2946,12 +2946,12 @@
       <c r="D107" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E107" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F107" s="43"/>
-      <c r="G107" s="43"/>
-      <c r="H107" s="43"/>
+      <c r="E107" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F107" s="45"/>
+      <c r="G107" s="45"/>
+      <c r="H107" s="45"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="20">
@@ -2963,12 +2963,12 @@
       <c r="D108" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E108" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F108" s="43"/>
-      <c r="G108" s="43"/>
-      <c r="H108" s="43"/>
+      <c r="E108" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F108" s="45"/>
+      <c r="G108" s="45"/>
+      <c r="H108" s="45"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="20">
@@ -2980,12 +2980,12 @@
       <c r="D109" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E109" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F109" s="43"/>
-      <c r="G109" s="43"/>
-      <c r="H109" s="43"/>
+      <c r="E109" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F109" s="45"/>
+      <c r="G109" s="45"/>
+      <c r="H109" s="45"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="20">
@@ -2997,12 +2997,12 @@
       <c r="D110" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E110" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F110" s="43"/>
-      <c r="G110" s="43"/>
-      <c r="H110" s="43"/>
+      <c r="E110" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F110" s="45"/>
+      <c r="G110" s="45"/>
+      <c r="H110" s="45"/>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="20">
@@ -3014,12 +3014,12 @@
       <c r="D111" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E111" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F111" s="43"/>
-      <c r="G111" s="43"/>
-      <c r="H111" s="43"/>
+      <c r="E111" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F111" s="45"/>
+      <c r="G111" s="45"/>
+      <c r="H111" s="45"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="20">
@@ -3031,12 +3031,12 @@
       <c r="D112" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E112" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F112" s="43"/>
-      <c r="G112" s="43"/>
-      <c r="H112" s="43"/>
+      <c r="E112" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F112" s="45"/>
+      <c r="G112" s="45"/>
+      <c r="H112" s="45"/>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B113" s="20">
@@ -3048,12 +3048,12 @@
       <c r="D113" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E113" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F113" s="43"/>
-      <c r="G113" s="43"/>
-      <c r="H113" s="43"/>
+      <c r="E113" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F113" s="45"/>
+      <c r="G113" s="45"/>
+      <c r="H113" s="45"/>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B114" s="20">
@@ -3065,12 +3065,12 @@
       <c r="D114" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E114" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F114" s="43"/>
-      <c r="G114" s="43"/>
-      <c r="H114" s="43"/>
+      <c r="E114" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F114" s="45"/>
+      <c r="G114" s="45"/>
+      <c r="H114" s="45"/>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B115" s="20">
@@ -3082,12 +3082,12 @@
       <c r="D115" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E115" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F115" s="43"/>
-      <c r="G115" s="43"/>
-      <c r="H115" s="43"/>
+      <c r="E115" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F115" s="45"/>
+      <c r="G115" s="45"/>
+      <c r="H115" s="45"/>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B116" s="9" t="s">
@@ -3099,12 +3099,12 @@
       <c r="D116" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E116" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F116" s="43"/>
-      <c r="G116" s="43"/>
-      <c r="H116" s="43"/>
+      <c r="E116" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F116" s="45"/>
+      <c r="G116" s="45"/>
+      <c r="H116" s="45"/>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B117" s="20">
@@ -3116,12 +3116,12 @@
       <c r="D117" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E117" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F117" s="43"/>
-      <c r="G117" s="43"/>
-      <c r="H117" s="43"/>
+      <c r="E117" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F117" s="45"/>
+      <c r="G117" s="45"/>
+      <c r="H117" s="45"/>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B118" s="20">
@@ -3133,12 +3133,12 @@
       <c r="D118" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E118" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F118" s="44"/>
-      <c r="G118" s="45"/>
-      <c r="H118" s="46"/>
+      <c r="E118" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" s="66"/>
+      <c r="G118" s="67"/>
+      <c r="H118" s="68"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B119" s="20">
@@ -3150,12 +3150,12 @@
       <c r="D119" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E119" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F119" s="44"/>
-      <c r="G119" s="45"/>
-      <c r="H119" s="46"/>
+      <c r="E119" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" s="66"/>
+      <c r="G119" s="67"/>
+      <c r="H119" s="68"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B120" s="20">
@@ -3167,12 +3167,12 @@
       <c r="D120" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E120" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F120" s="44"/>
-      <c r="G120" s="45"/>
-      <c r="H120" s="46"/>
+      <c r="E120" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F120" s="66"/>
+      <c r="G120" s="67"/>
+      <c r="H120" s="68"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B121" s="20">
@@ -3184,12 +3184,12 @@
       <c r="D121" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E121" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F121" s="43"/>
-      <c r="G121" s="43"/>
-      <c r="H121" s="43"/>
+      <c r="E121" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F121" s="45"/>
+      <c r="G121" s="45"/>
+      <c r="H121" s="45"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B122" s="20">
@@ -3201,12 +3201,12 @@
       <c r="D122" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E122" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F122" s="43"/>
-      <c r="G122" s="43"/>
-      <c r="H122" s="43"/>
+      <c r="E122" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F122" s="45"/>
+      <c r="G122" s="45"/>
+      <c r="H122" s="45"/>
       <c r="J122" s="10" t="s">
         <v>38</v>
       </c>
@@ -3221,12 +3221,12 @@
       <c r="D123" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E123" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F123" s="43"/>
-      <c r="G123" s="43"/>
-      <c r="H123" s="43"/>
+      <c r="E123" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F123" s="45"/>
+      <c r="G123" s="45"/>
+      <c r="H123" s="45"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B124" s="20">
@@ -3241,9 +3241,9 @@
       <c r="E124" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F124" s="43"/>
-      <c r="G124" s="43"/>
-      <c r="H124" s="43"/>
+      <c r="F124" s="45"/>
+      <c r="G124" s="45"/>
+      <c r="H124" s="45"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B125" s="20">
@@ -3258,9 +3258,9 @@
       <c r="E125" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F125" s="43"/>
-      <c r="G125" s="43"/>
-      <c r="H125" s="43"/>
+      <c r="F125" s="45"/>
+      <c r="G125" s="45"/>
+      <c r="H125" s="45"/>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B126" s="20">
@@ -3275,9 +3275,9 @@
       <c r="E126" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F126" s="43"/>
-      <c r="G126" s="43"/>
-      <c r="H126" s="43"/>
+      <c r="F126" s="45"/>
+      <c r="G126" s="45"/>
+      <c r="H126" s="45"/>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B127" s="20">
@@ -3292,9 +3292,9 @@
       <c r="E127" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F127" s="43"/>
-      <c r="G127" s="43"/>
-      <c r="H127" s="43"/>
+      <c r="F127" s="45"/>
+      <c r="G127" s="45"/>
+      <c r="H127" s="45"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B128" s="20">
@@ -3309,9 +3309,9 @@
       <c r="E128" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F128" s="43"/>
-      <c r="G128" s="43"/>
-      <c r="H128" s="43"/>
+      <c r="F128" s="45"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="45"/>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="20">
@@ -3326,9 +3326,9 @@
       <c r="E129" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F129" s="43"/>
-      <c r="G129" s="43"/>
-      <c r="H129" s="43"/>
+      <c r="F129" s="45"/>
+      <c r="G129" s="45"/>
+      <c r="H129" s="45"/>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="20">
@@ -3343,9 +3343,9 @@
       <c r="E130" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F130" s="43"/>
-      <c r="G130" s="43"/>
-      <c r="H130" s="43"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="45"/>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="20">
@@ -3360,9 +3360,9 @@
       <c r="E131" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F131" s="43"/>
-      <c r="G131" s="43"/>
-      <c r="H131" s="43"/>
+      <c r="F131" s="45"/>
+      <c r="G131" s="45"/>
+      <c r="H131" s="45"/>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="20">
@@ -3377,9 +3377,9 @@
       <c r="E132" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F132" s="43"/>
-      <c r="G132" s="43"/>
-      <c r="H132" s="43"/>
+      <c r="F132" s="45"/>
+      <c r="G132" s="45"/>
+      <c r="H132" s="45"/>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="20">
@@ -3394,9 +3394,9 @@
       <c r="E133" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F133" s="43"/>
-      <c r="G133" s="43"/>
-      <c r="H133" s="43"/>
+      <c r="F133" s="45"/>
+      <c r="G133" s="45"/>
+      <c r="H133" s="45"/>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="20">
@@ -3411,9 +3411,9 @@
       <c r="E134" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F134" s="43"/>
-      <c r="G134" s="43"/>
-      <c r="H134" s="43"/>
+      <c r="F134" s="45"/>
+      <c r="G134" s="45"/>
+      <c r="H134" s="45"/>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="20">
@@ -3428,9 +3428,9 @@
       <c r="E135" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F135" s="43"/>
-      <c r="G135" s="43"/>
-      <c r="H135" s="43"/>
+      <c r="F135" s="45"/>
+      <c r="G135" s="45"/>
+      <c r="H135" s="45"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" s="20">
@@ -3445,9 +3445,9 @@
       <c r="E136" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F136" s="43"/>
-      <c r="G136" s="43"/>
-      <c r="H136" s="43"/>
+      <c r="F136" s="45"/>
+      <c r="G136" s="45"/>
+      <c r="H136" s="45"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" s="20">
@@ -3462,9 +3462,9 @@
       <c r="E137" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F137" s="43"/>
-      <c r="G137" s="43"/>
-      <c r="H137" s="43"/>
+      <c r="F137" s="45"/>
+      <c r="G137" s="45"/>
+      <c r="H137" s="45"/>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="20">
@@ -3479,9 +3479,9 @@
       <c r="E138" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F138" s="43"/>
-      <c r="G138" s="43"/>
-      <c r="H138" s="43"/>
+      <c r="F138" s="45"/>
+      <c r="G138" s="45"/>
+      <c r="H138" s="45"/>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="20">
@@ -3496,9 +3496,9 @@
       <c r="E139" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F139" s="43"/>
-      <c r="G139" s="43"/>
-      <c r="H139" s="43"/>
+      <c r="F139" s="45"/>
+      <c r="G139" s="45"/>
+      <c r="H139" s="45"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" s="20">
@@ -3513,9 +3513,9 @@
       <c r="E140" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F140" s="43"/>
-      <c r="G140" s="43"/>
-      <c r="H140" s="43"/>
+      <c r="F140" s="45"/>
+      <c r="G140" s="45"/>
+      <c r="H140" s="45"/>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="20">
@@ -3530,9 +3530,9 @@
       <c r="E141" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F141" s="43"/>
-      <c r="G141" s="43"/>
-      <c r="H141" s="43"/>
+      <c r="F141" s="45"/>
+      <c r="G141" s="45"/>
+      <c r="H141" s="45"/>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="20">
@@ -3547,13 +3547,101 @@
       <c r="E142" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F142" s="43"/>
-      <c r="G142" s="43"/>
-      <c r="H142" s="43"/>
+      <c r="F142" s="45"/>
+      <c r="G142" s="45"/>
+      <c r="H142" s="45"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="lCPgoHp4bLbIL1JNSK1ttH4+ZWvchbvc6Q2GSYOJu0YqXyyM/lw16pZxohXMjvCxn31f3hDIG8XQ3rUZmvOdDA==" saltValue="q8lea4feKY9l39UvYwa3nA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="112">
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C68:G68"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C61:G61"/>
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="F140:H140"/>
@@ -3578,94 +3666,6 @@
     <mergeCell ref="F83:H83"/>
     <mergeCell ref="F84:H84"/>
     <mergeCell ref="F85:H85"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>